<commit_message>
Updated README.md. Updated PAS documents to match synced files as of 10.27.24
</commit_message>
<xml_diff>
--- a/ParkingAvailabilitySystem-Documents/ContributionLog.xlsx
+++ b/ParkingAvailabilitySystem-Documents/ContributionLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/emeurrens_ufl_edu/Documents/parking-availability-system/ParkingAvailabilitySystem-Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75995CFB-CB0E-B148-A8C2-9F28FC844F00}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D377A8A7-B77A-4413-B3C3-04DBF39D7083}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contrib-log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>PAS Contribution Log</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t xml:space="preserve">Raspberry pi is capable of reading from table schemas in the database, writing to the database (also capable of creating tables), and interacting with an installed camera module to take pictures. </t>
+  </si>
+  <si>
+    <t>Raspberry Pi remote configuration</t>
+  </si>
+  <si>
+    <t>Configured SSH/VNC and Jupyter Notebook to be able to access board, using the UF VPN, while it is connected to the UF WiFi network</t>
   </si>
 </sst>
 </file>
@@ -504,19 +510,19 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.75390625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.76953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.55078125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="11.109375" style="1" customWidth="1"/>
     <col min="27" max="27" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -525,7 +531,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -534,7 +540,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:27" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
@@ -543,7 +549,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -563,7 +569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -578,7 +584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -592,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -606,12 +612,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4">
+        <v>45580</v>
+      </c>
+      <c r="E8" s="4">
+        <v>45585</v>
+      </c>
       <c r="AA8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="AA9" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Added project assignment files up to 02/05/2025
</commit_message>
<xml_diff>
--- a/ParkingAvailabilitySystem-Documents/ContributionLog.xlsx
+++ b/ParkingAvailabilitySystem-Documents/ContributionLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/emeurrens_ufl_edu/Documents/parking-availability-system/ParkingAvailabilitySystem-Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D377A8A7-B77A-4413-B3C3-04DBF39D7083}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="11_F25DC773A252ABDACC10484CE1DF4FE65ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CE4E2D6-C9EC-43EB-AE66-C8DD4E04865A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>PAS Contribution Log</t>
   </si>
@@ -65,43 +65,52 @@
     <t>Member Names</t>
   </si>
   <si>
+    <t>Benjamin Simonson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry pi configuration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspian loaded onto the boot SD card and raspberry pi boots properly </t>
+  </si>
+  <si>
     <t>Erik Meurrens</t>
   </si>
   <si>
-    <t>Benjamin Simonson</t>
+    <t xml:space="preserve">Raspberry pi connection to the PostgreSQL database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry pi established connection to the database successfully by referencing secrets stored securely on the device. </t>
+  </si>
+  <si>
+    <t>Raspberry pi read, write, and pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry pi is capable of reading from table schemas in the database, writing to the database (also capable of creating tables), and interacting with an installed camera module to take pictures. </t>
   </si>
   <si>
     <t>Ryan Jalloul</t>
   </si>
   <si>
+    <t>Raspberry Pi remote configuration</t>
+  </si>
+  <si>
+    <t>Configured SSH/VNC and Jupyter Notebook to be able to access board, using the UF VPN, while it is connected to the UF WiFi network</t>
+  </si>
+  <si>
     <t>Evan Tobon</t>
   </si>
   <si>
     <t>Samer Khatib</t>
   </si>
   <si>
-    <t xml:space="preserve">Raspberry pi configuration </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspian loaded onto the boot SD card and raspberry pi boots properly </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry pi connection to the PostgreSQL database </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry pi established connection to the database successfully by referencing secrets stored securely on the device. </t>
-  </si>
-  <si>
-    <t>Raspberry pi read, write, and pictures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry pi is capable of reading from table schemas in the database, writing to the database (also capable of creating tables), and interacting with an installed camera module to take pictures. </t>
-  </si>
-  <si>
-    <t>Raspberry Pi remote configuration</t>
-  </si>
-  <si>
-    <t>Configured SSH/VNC and Jupyter Notebook to be able to access board, using the UF VPN, while it is connected to the UF WiFi network</t>
+    <t>Garage networking</t>
+  </si>
+  <si>
+    <t>Investigating solutions to solving WiFi deadzone issue within garage. Looking into hardware that can be used to act as a network access point for the UF network.</t>
+  </si>
+  <si>
+    <t>RPi configuration script</t>
   </si>
 </sst>
 </file>
@@ -242,6 +251,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,16 +520,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
     <col min="4" max="5" width="11.109375" style="1" customWidth="1"/>
     <col min="27" max="27" width="0" hidden="1" customWidth="1"/>
@@ -571,56 +584,56 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4"/>
       <c r="AA5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AA6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AA7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4">
         <v>45580</v>
@@ -629,12 +642,43 @@
         <v>45585</v>
       </c>
       <c r="AA8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45676</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45681</v>
+      </c>
       <c r="AA9" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>